<commit_message>
Update Sprint Burndown Chart.xlsx
</commit_message>
<xml_diff>
--- a/Concepts/Scrum/Sprint Burndown Chart.xlsx
+++ b/Concepts/Scrum/Sprint Burndown Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a36f19f9f59381e3/Development/Java/Vokabeltrainer/Concepts/Scrum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adria\Documents\.Workspace_Adrian_Java\Vokabeltrainer\Concepts\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{67C303B6-F0B5-4BA1-8CC4-2B11A4C0F4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ADB9BCB-D872-46E0-9C3B-790AE3BE44A1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E3F68E-BD1E-4E7E-870D-3CC3027622E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7515D94D-545D-4182-8278-535D5E64474B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{7515D94D-545D-4182-8278-535D5E64474B}"/>
   </bookViews>
   <sheets>
     <sheet name="Vokabeltrainer Sprint 1" sheetId="1" r:id="rId1"/>
@@ -361,10 +361,10 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2731,20 +2731,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA7647-D963-4853-AAC1-D89A10D34152}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.46484375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.46484375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.46484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -2772,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5">
@@ -2785,7 +2785,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <v>44986</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <v>45000</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <v>45014</v>
       </c>
@@ -2834,13 +2834,15 @@
         <f t="shared" ref="C6:E6" si="0">C5-B6</f>
         <v>10</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
         <v>45042</v>
       </c>
@@ -2851,13 +2853,15 @@
         <f t="shared" ref="C7" si="1">C6-B7</f>
         <v>0</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>10</v>
+      </c>
       <c r="E7" s="5">
         <f t="shared" ref="E7" si="2">E6-D7</f>
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
     </row>
   </sheetData>
@@ -2878,20 +2882,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7512A0E2-CA00-4A05-A389-68BE8FA72B29}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.46484375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.46484375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.46484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2904,7 +2908,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -2919,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5">
@@ -2932,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <v>45070</v>
       </c>
@@ -2947,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <v>45098</v>
       </c>
@@ -2962,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <v>45112</v>
       </c>
@@ -2977,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
     </row>
   </sheetData>

</xml_diff>